<commit_message>
Excel changed with dichotomic variable
</commit_message>
<xml_diff>
--- a/ejemplo_supervivencia.xlsx
+++ b/ejemplo_supervivencia.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\R\SurvApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB9F74-DE44-42B6-8FBE-003BAD6B9DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NumPac</t>
   </si>
@@ -27,15 +33,18 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>VarDic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,29 +92,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +174,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -177,6 +208,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -211,9 +243,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,14 +419,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +441,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -420,8 +458,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -434,8 +475,11 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -448,8 +492,11 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -462,8 +509,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -476,8 +526,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -490,8 +543,11 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -504,8 +560,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -518,8 +577,11 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -532,8 +594,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -546,8 +611,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -560,8 +628,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -574,8 +645,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -588,8 +662,11 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -602,8 +679,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -616,8 +696,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -630,8 +713,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -644,8 +730,11 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -658,8 +747,11 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -672,8 +764,11 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -686,8 +781,11 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -700,8 +798,11 @@
       <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -714,8 +815,11 @@
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -728,8 +832,11 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -742,8 +849,11 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -756,8 +866,11 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -770,8 +883,11 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -784,8 +900,11 @@
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -798,8 +917,11 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -812,8 +934,11 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -826,8 +951,11 @@
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -840,8 +968,11 @@
       <c r="D32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -854,8 +985,11 @@
       <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -868,8 +1002,11 @@
       <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -882,8 +1019,11 @@
       <c r="D35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -896,8 +1036,11 @@
       <c r="D36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -910,8 +1053,11 @@
       <c r="D37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -924,8 +1070,11 @@
       <c r="D38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -938,8 +1087,11 @@
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -952,8 +1104,11 @@
       <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -966,8 +1121,11 @@
       <c r="D41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -980,8 +1138,11 @@
       <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -994,8 +1155,11 @@
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1008,8 +1172,11 @@
       <c r="D44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1022,8 +1189,11 @@
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1036,8 +1206,11 @@
       <c r="D46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1050,8 +1223,11 @@
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1064,8 +1240,11 @@
       <c r="D48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1078,8 +1257,11 @@
       <c r="D49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1092,8 +1274,11 @@
       <c r="D50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1106,8 +1291,11 @@
       <c r="D51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1120,8 +1308,11 @@
       <c r="D52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1134,8 +1325,11 @@
       <c r="D53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1148,8 +1342,11 @@
       <c r="D54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1162,8 +1359,11 @@
       <c r="D55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1176,8 +1376,11 @@
       <c r="D56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1190,8 +1393,11 @@
       <c r="D57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1204,8 +1410,11 @@
       <c r="D58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1218,8 +1427,11 @@
       <c r="D59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1232,8 +1444,11 @@
       <c r="D60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1246,8 +1461,11 @@
       <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1260,8 +1478,11 @@
       <c r="D62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1274,8 +1495,11 @@
       <c r="D63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1288,8 +1512,11 @@
       <c r="D64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1302,8 +1529,11 @@
       <c r="D65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1316,8 +1546,11 @@
       <c r="D66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1330,8 +1563,11 @@
       <c r="D67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1344,8 +1580,11 @@
       <c r="D68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1358,8 +1597,11 @@
       <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1372,8 +1614,11 @@
       <c r="D70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1386,8 +1631,11 @@
       <c r="D71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1400,8 +1648,11 @@
       <c r="D72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1414,8 +1665,11 @@
       <c r="D73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1428,8 +1682,11 @@
       <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1442,8 +1699,11 @@
       <c r="D75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1456,8 +1716,11 @@
       <c r="D76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1470,8 +1733,11 @@
       <c r="D77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1484,8 +1750,11 @@
       <c r="D78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1498,8 +1767,11 @@
       <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1512,8 +1784,11 @@
       <c r="D80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1526,8 +1801,11 @@
       <c r="D81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1540,8 +1818,11 @@
       <c r="D82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1554,8 +1835,11 @@
       <c r="D83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1568,8 +1852,11 @@
       <c r="D84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1582,8 +1869,11 @@
       <c r="D85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1596,8 +1886,11 @@
       <c r="D86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1610,8 +1903,11 @@
       <c r="D87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1624,8 +1920,11 @@
       <c r="D88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1638,8 +1937,11 @@
       <c r="D89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1652,8 +1954,11 @@
       <c r="D90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1666,8 +1971,11 @@
       <c r="D91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1680,8 +1988,11 @@
       <c r="D92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1694,8 +2005,11 @@
       <c r="D93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1708,8 +2022,11 @@
       <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1722,8 +2039,11 @@
       <c r="D95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1736,8 +2056,11 @@
       <c r="D96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1750,8 +2073,11 @@
       <c r="D97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1764,8 +2090,11 @@
       <c r="D98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1778,8 +2107,11 @@
       <c r="D99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1792,8 +2124,11 @@
       <c r="D100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -1806,8 +2141,11 @@
       <c r="D101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -1820,8 +2158,11 @@
       <c r="D102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -1834,8 +2175,11 @@
       <c r="D103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -1848,8 +2192,11 @@
       <c r="D104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -1862,8 +2209,11 @@
       <c r="D105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -1876,8 +2226,11 @@
       <c r="D106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -1890,8 +2243,11 @@
       <c r="D107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -1904,8 +2260,11 @@
       <c r="D108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -1918,8 +2277,11 @@
       <c r="D109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -1932,8 +2294,11 @@
       <c r="D110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -1946,8 +2311,11 @@
       <c r="D111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -1960,8 +2328,11 @@
       <c r="D112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -1974,8 +2345,11 @@
       <c r="D113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -1988,8 +2362,11 @@
       <c r="D114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2002,8 +2379,11 @@
       <c r="D115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2016,8 +2396,11 @@
       <c r="D116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2030,8 +2413,11 @@
       <c r="D117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2044,8 +2430,11 @@
       <c r="D118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2058,8 +2447,11 @@
       <c r="D119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2072,8 +2464,11 @@
       <c r="D120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2084,6 +2479,9 @@
         <v>43559</v>
       </c>
       <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
         <v>0</v>
       </c>
     </row>

</xml_diff>